<commit_message>
Update GMM and Other Solvers
</commit_message>
<xml_diff>
--- a/experiments/experiment5/ComparativeAnalysis.xlsx
+++ b/experiments/experiment5/ComparativeAnalysis.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2832,68 +2829,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="D3">
-            <v>-6.3294444444444444</v>
-          </cell>
-          <cell r="J3">
-            <v>-6.217222221914998</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>-5.9988095238095243</v>
-          </cell>
-          <cell r="J4">
-            <v>-5.9421428568044892</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>-5.9457936507936484</v>
-          </cell>
-          <cell r="J5">
-            <v>-5.8796693113413268</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>-5.8776689051689042</v>
-          </cell>
-          <cell r="J6">
-            <v>-5.7912313584908723</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>-5.8153607503607478</v>
-          </cell>
-          <cell r="J7">
-            <v>-5.7128929357513583</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>-5.631833054859368</v>
-          </cell>
-          <cell r="J8">
-            <v>-5.5241773894266313</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3193,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>